<commit_message>
Send Data ergänzt,  accept Data fehlt noch
</commit_message>
<xml_diff>
--- a/Doku/KnxNetIp-Protokoll.xlsx
+++ b/Doku/KnxNetIp-Protokoll.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="150" windowWidth="18915" windowHeight="12330" activeTab="6"/>
+    <workbookView xWindow="360" yWindow="150" windowWidth="18915" windowHeight="12330" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="ConReq" sheetId="1" r:id="rId1"/>
@@ -14,14 +14,15 @@
     <sheet name="HBReq" sheetId="7" r:id="rId5"/>
     <sheet name="HBResp" sheetId="8" r:id="rId6"/>
     <sheet name="Data" sheetId="9" r:id="rId7"/>
-    <sheet name="Tabelle3" sheetId="3" r:id="rId8"/>
+    <sheet name="DataSend" sheetId="10" r:id="rId8"/>
+    <sheet name="Tabelle3" sheetId="3" r:id="rId9"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="64">
   <si>
     <t>1A</t>
   </si>
@@ -227,6 +228,21 @@
   </si>
   <si>
     <t>xx</t>
+  </si>
+  <si>
+    <t>Null</t>
+  </si>
+  <si>
+    <t>Send Data</t>
+  </si>
+  <si>
+    <t>Receive Data</t>
+  </si>
+  <si>
+    <t>Disconnection Response</t>
+  </si>
+  <si>
+    <t>MSG Code   0x11 = L_Data.req</t>
   </si>
 </sst>
 </file>
@@ -345,7 +361,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
@@ -397,14 +413,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -419,13 +429,22 @@
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -730,7 +749,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:E31"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E14" sqref="E14:E19"/>
     </sheetView>
   </sheetViews>
@@ -750,10 +769,10 @@
       </c>
     </row>
     <row r="5" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="24" t="s">
+      <c r="A5" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="24"/>
+      <c r="B5" s="22"/>
       <c r="C5" s="6" t="s">
         <v>4</v>
       </c>
@@ -772,7 +791,7 @@
       <c r="C6" s="1">
         <v>6</v>
       </c>
-      <c r="D6" s="25" t="s">
+      <c r="D6" s="23" t="s">
         <v>8</v>
       </c>
       <c r="E6" s="5" t="s">
@@ -790,7 +809,7 @@
       <c r="C7" s="1">
         <v>10</v>
       </c>
-      <c r="D7" s="26"/>
+      <c r="D7" s="24"/>
       <c r="E7" s="5" t="s">
         <v>31</v>
       </c>
@@ -806,8 +825,8 @@
       <c r="C8" s="1">
         <v>2</v>
       </c>
-      <c r="D8" s="26"/>
-      <c r="E8" s="21" t="s">
+      <c r="D8" s="24"/>
+      <c r="E8" s="27" t="s">
         <v>32</v>
       </c>
     </row>
@@ -822,8 +841,8 @@
       <c r="C9" s="1">
         <v>5</v>
       </c>
-      <c r="D9" s="26"/>
-      <c r="E9" s="22"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="28"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -836,8 +855,8 @@
       <c r="C10" s="1">
         <v>0</v>
       </c>
-      <c r="D10" s="26"/>
-      <c r="E10" s="23" t="s">
+      <c r="D10" s="24"/>
+      <c r="E10" s="29" t="s">
         <v>18</v>
       </c>
     </row>
@@ -852,8 +871,8 @@
       <c r="C11" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D11" s="27"/>
-      <c r="E11" s="22"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="28"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -866,7 +885,7 @@
       <c r="C12" s="1">
         <v>8</v>
       </c>
-      <c r="D12" s="25" t="s">
+      <c r="D12" s="23" t="s">
         <v>9</v>
       </c>
       <c r="E12" s="5" t="s">
@@ -884,7 +903,7 @@
       <c r="C13" s="1">
         <v>1</v>
       </c>
-      <c r="D13" s="26"/>
+      <c r="D13" s="24"/>
       <c r="E13" s="5" t="s">
         <v>33</v>
       </c>
@@ -900,8 +919,8 @@
       <c r="C14" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D14" s="26"/>
-      <c r="E14" s="20" t="s">
+      <c r="D14" s="24"/>
+      <c r="E14" s="26" t="s">
         <v>12</v>
       </c>
     </row>
@@ -916,8 +935,8 @@
       <c r="C15" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D15" s="26"/>
-      <c r="E15" s="20"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="26"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
@@ -930,8 +949,8 @@
       <c r="C16" s="1">
         <v>0</v>
       </c>
-      <c r="D16" s="26"/>
-      <c r="E16" s="20"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="26"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
@@ -944,8 +963,8 @@
       <c r="C17" s="1">
         <v>12</v>
       </c>
-      <c r="D17" s="26"/>
-      <c r="E17" s="20"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="26"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
@@ -958,8 +977,8 @@
       <c r="C18" s="1">
         <v>46</v>
       </c>
-      <c r="D18" s="26"/>
-      <c r="E18" s="20" t="s">
+      <c r="D18" s="24"/>
+      <c r="E18" s="26" t="s">
         <v>13</v>
       </c>
     </row>
@@ -974,8 +993,8 @@
       <c r="C19" s="1">
         <v>51</v>
       </c>
-      <c r="D19" s="27"/>
-      <c r="E19" s="20"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="26"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
@@ -988,7 +1007,7 @@
       <c r="C20" s="1">
         <v>8</v>
       </c>
-      <c r="D20" s="25" t="s">
+      <c r="D20" s="23" t="s">
         <v>10</v>
       </c>
       <c r="E20" s="5" t="s">
@@ -1006,7 +1025,7 @@
       <c r="C21" s="1">
         <v>1</v>
       </c>
-      <c r="D21" s="26"/>
+      <c r="D21" s="24"/>
       <c r="E21" s="5" t="s">
         <v>33</v>
       </c>
@@ -1022,8 +1041,8 @@
       <c r="C22" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D22" s="26"/>
-      <c r="E22" s="20" t="s">
+      <c r="D22" s="24"/>
+      <c r="E22" s="26" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1038,8 +1057,8 @@
       <c r="C23" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D23" s="26"/>
-      <c r="E23" s="20"/>
+      <c r="D23" s="24"/>
+      <c r="E23" s="26"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
@@ -1052,8 +1071,8 @@
       <c r="C24" s="1">
         <v>0</v>
       </c>
-      <c r="D24" s="26"/>
-      <c r="E24" s="20"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="26"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
@@ -1066,8 +1085,8 @@
       <c r="C25" s="1">
         <v>12</v>
       </c>
-      <c r="D25" s="26"/>
-      <c r="E25" s="20"/>
+      <c r="D25" s="24"/>
+      <c r="E25" s="26"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
@@ -1080,8 +1099,8 @@
       <c r="C26" s="1">
         <v>46</v>
       </c>
-      <c r="D26" s="26"/>
-      <c r="E26" s="20" t="s">
+      <c r="D26" s="24"/>
+      <c r="E26" s="26" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1096,8 +1115,8 @@
       <c r="C27" s="1">
         <v>51</v>
       </c>
-      <c r="D27" s="27"/>
-      <c r="E27" s="20"/>
+      <c r="D27" s="25"/>
+      <c r="E27" s="26"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
@@ -1110,7 +1129,7 @@
       <c r="C28" s="1">
         <v>4</v>
       </c>
-      <c r="D28" s="26" t="s">
+      <c r="D28" s="24" t="s">
         <v>11</v>
       </c>
       <c r="E28" s="5" t="s">
@@ -1128,7 +1147,7 @@
       <c r="C29" s="1">
         <v>4</v>
       </c>
-      <c r="D29" s="26"/>
+      <c r="D29" s="24"/>
       <c r="E29" s="5" t="s">
         <v>20</v>
       </c>
@@ -1144,7 +1163,7 @@
       <c r="C30" s="1">
         <v>2</v>
       </c>
-      <c r="D30" s="26"/>
+      <c r="D30" s="24"/>
       <c r="E30" s="5" t="s">
         <v>19</v>
       </c>
@@ -1160,24 +1179,24 @@
       <c r="C31" s="1">
         <v>0</v>
       </c>
-      <c r="D31" s="27"/>
+      <c r="D31" s="25"/>
       <c r="E31" s="5" t="s">
         <v>21</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="D6:D11"/>
-    <mergeCell ref="D12:D19"/>
-    <mergeCell ref="D20:D27"/>
-    <mergeCell ref="D28:D31"/>
     <mergeCell ref="E14:E17"/>
     <mergeCell ref="E18:E19"/>
     <mergeCell ref="E22:E25"/>
     <mergeCell ref="E26:E27"/>
     <mergeCell ref="E8:E9"/>
     <mergeCell ref="E10:E11"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="D6:D11"/>
+    <mergeCell ref="D12:D19"/>
+    <mergeCell ref="D20:D27"/>
+    <mergeCell ref="D28:D31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1187,7 +1206,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:L31"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D12" sqref="D12:E13"/>
     </sheetView>
   </sheetViews>
@@ -1207,10 +1226,10 @@
       </c>
     </row>
     <row r="5" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="24" t="s">
+      <c r="A5" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="24"/>
+      <c r="B5" s="22"/>
       <c r="C5" s="6" t="s">
         <v>4</v>
       </c>
@@ -1229,7 +1248,7 @@
       <c r="C6" s="1">
         <v>6</v>
       </c>
-      <c r="D6" s="25" t="s">
+      <c r="D6" s="23" t="s">
         <v>8</v>
       </c>
       <c r="E6" s="5" t="s">
@@ -1247,7 +1266,7 @@
       <c r="C7" s="1">
         <v>10</v>
       </c>
-      <c r="D7" s="26"/>
+      <c r="D7" s="24"/>
       <c r="E7" s="5" t="s">
         <v>17</v>
       </c>
@@ -1263,8 +1282,8 @@
       <c r="C8" s="1">
         <v>2</v>
       </c>
-      <c r="D8" s="26"/>
-      <c r="E8" s="21" t="s">
+      <c r="D8" s="24"/>
+      <c r="E8" s="27" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1279,8 +1298,8 @@
       <c r="C9" s="1">
         <v>6</v>
       </c>
-      <c r="D9" s="26"/>
-      <c r="E9" s="22"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="28"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -1293,8 +1312,8 @@
       <c r="C10" s="1">
         <v>0</v>
       </c>
-      <c r="D10" s="26"/>
-      <c r="E10" s="23" t="s">
+      <c r="D10" s="24"/>
+      <c r="E10" s="29" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1309,8 +1328,8 @@
       <c r="C11" s="1">
         <v>14</v>
       </c>
-      <c r="D11" s="27"/>
-      <c r="E11" s="22"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="28"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -1359,7 +1378,7 @@
       <c r="C14" s="1">
         <v>8</v>
       </c>
-      <c r="D14" s="25" t="s">
+      <c r="D14" s="23" t="s">
         <v>9</v>
       </c>
       <c r="E14" s="5" t="s">
@@ -1377,7 +1396,7 @@
       <c r="C15" s="1">
         <v>1</v>
       </c>
-      <c r="D15" s="26"/>
+      <c r="D15" s="24"/>
       <c r="E15" s="5" t="s">
         <v>33</v>
       </c>
@@ -1393,8 +1412,8 @@
       <c r="C16" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D16" s="26"/>
-      <c r="E16" s="20" t="s">
+      <c r="D16" s="24"/>
+      <c r="E16" s="26" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1409,8 +1428,8 @@
       <c r="C17" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D17" s="26"/>
-      <c r="E17" s="20"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="26"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18">
@@ -1423,8 +1442,8 @@
       <c r="C18" s="1">
         <v>0</v>
       </c>
-      <c r="D18" s="26"/>
-      <c r="E18" s="20"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="26"/>
       <c r="H18" s="13"/>
       <c r="I18" s="13"/>
       <c r="J18" s="13"/>
@@ -1442,8 +1461,8 @@
       <c r="C19" s="1">
         <v>3</v>
       </c>
-      <c r="D19" s="26"/>
-      <c r="E19" s="20"/>
+      <c r="D19" s="24"/>
+      <c r="E19" s="26"/>
       <c r="H19" s="13"/>
       <c r="I19" s="13"/>
       <c r="J19" s="13"/>
@@ -1461,8 +1480,8 @@
       <c r="C20" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D20" s="26"/>
-      <c r="E20" s="20" t="s">
+      <c r="D20" s="24"/>
+      <c r="E20" s="26" t="s">
         <v>29</v>
       </c>
       <c r="H20" s="13"/>
@@ -1482,8 +1501,8 @@
       <c r="C21" s="1">
         <v>57</v>
       </c>
-      <c r="D21" s="27"/>
-      <c r="E21" s="20"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="26"/>
       <c r="H21" s="13"/>
       <c r="I21" s="13"/>
       <c r="J21" s="13"/>
@@ -1501,7 +1520,7 @@
       <c r="C22" s="1">
         <v>4</v>
       </c>
-      <c r="D22" s="26" t="s">
+      <c r="D22" s="24" t="s">
         <v>11</v>
       </c>
       <c r="E22" s="5" t="s">
@@ -1524,7 +1543,7 @@
       <c r="C23" s="1">
         <v>4</v>
       </c>
-      <c r="D23" s="26"/>
+      <c r="D23" s="24"/>
       <c r="E23" s="5" t="s">
         <v>20</v>
       </c>
@@ -1545,7 +1564,7 @@
       <c r="C24" s="1">
         <v>11</v>
       </c>
-      <c r="D24" s="26"/>
+      <c r="D24" s="24"/>
       <c r="E24" s="5" t="s">
         <v>34</v>
       </c>
@@ -1566,7 +1585,7 @@
       <c r="C25" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D25" s="27"/>
+      <c r="D25" s="25"/>
       <c r="E25" s="5" t="s">
         <v>21</v>
       </c>
@@ -1644,10 +1663,10 @@
       </c>
     </row>
     <row r="5" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="24" t="s">
+      <c r="A5" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="24"/>
+      <c r="B5" s="22"/>
       <c r="C5" s="6" t="s">
         <v>4</v>
       </c>
@@ -1666,7 +1685,7 @@
       <c r="C6" s="1">
         <v>6</v>
       </c>
-      <c r="D6" s="25" t="s">
+      <c r="D6" s="23" t="s">
         <v>8</v>
       </c>
       <c r="E6" s="5" t="s">
@@ -1684,7 +1703,7 @@
       <c r="C7" s="1">
         <v>10</v>
       </c>
-      <c r="D7" s="26"/>
+      <c r="D7" s="24"/>
       <c r="E7" s="5" t="s">
         <v>31</v>
       </c>
@@ -1700,8 +1719,8 @@
       <c r="C8" s="1">
         <v>2</v>
       </c>
-      <c r="D8" s="26"/>
-      <c r="E8" s="21" t="s">
+      <c r="D8" s="24"/>
+      <c r="E8" s="27" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1716,8 +1735,8 @@
       <c r="C9" s="1">
         <v>9</v>
       </c>
-      <c r="D9" s="26"/>
-      <c r="E9" s="22"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="28"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -1730,8 +1749,8 @@
       <c r="C10" s="1">
         <v>0</v>
       </c>
-      <c r="D10" s="26"/>
-      <c r="E10" s="23" t="s">
+      <c r="D10" s="24"/>
+      <c r="E10" s="29" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1746,8 +1765,8 @@
       <c r="C11" s="1">
         <v>10</v>
       </c>
-      <c r="D11" s="27"/>
-      <c r="E11" s="22"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="28"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -1796,7 +1815,7 @@
       <c r="C14" s="1">
         <v>8</v>
       </c>
-      <c r="D14" s="28" t="s">
+      <c r="D14" s="30" t="s">
         <v>9</v>
       </c>
       <c r="E14" s="5" t="s">
@@ -1814,7 +1833,7 @@
       <c r="C15" s="1">
         <v>1</v>
       </c>
-      <c r="D15" s="28"/>
+      <c r="D15" s="30"/>
       <c r="E15" s="5" t="s">
         <v>33</v>
       </c>
@@ -1830,8 +1849,8 @@
       <c r="C16" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D16" s="28"/>
-      <c r="E16" s="20" t="s">
+      <c r="D16" s="30"/>
+      <c r="E16" s="26" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1846,8 +1865,8 @@
       <c r="C17" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D17" s="28"/>
-      <c r="E17" s="20"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="26"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
@@ -1860,8 +1879,8 @@
       <c r="C18" s="1">
         <v>0</v>
       </c>
-      <c r="D18" s="28"/>
-      <c r="E18" s="20"/>
+      <c r="D18" s="30"/>
+      <c r="E18" s="26"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
@@ -1874,8 +1893,8 @@
       <c r="C19" s="1">
         <v>12</v>
       </c>
-      <c r="D19" s="28"/>
-      <c r="E19" s="20"/>
+      <c r="D19" s="30"/>
+      <c r="E19" s="26"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
@@ -1888,8 +1907,8 @@
       <c r="C20" s="1">
         <v>46</v>
       </c>
-      <c r="D20" s="28"/>
-      <c r="E20" s="20" t="s">
+      <c r="D20" s="30"/>
+      <c r="E20" s="26" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1904,8 +1923,8 @@
       <c r="C21" s="1">
         <v>51</v>
       </c>
-      <c r="D21" s="28"/>
-      <c r="E21" s="20"/>
+      <c r="D21" s="30"/>
+      <c r="E21" s="26"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="8"/>
@@ -1978,7 +1997,7 @@
   <dimension ref="A3:L31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1993,14 +2012,14 @@
   <sheetData>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>22</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="24" t="s">
+      <c r="A5" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="24"/>
+      <c r="B5" s="22"/>
       <c r="C5" s="6" t="s">
         <v>4</v>
       </c>
@@ -2019,7 +2038,7 @@
       <c r="C6" s="1">
         <v>6</v>
       </c>
-      <c r="D6" s="25" t="s">
+      <c r="D6" s="23" t="s">
         <v>8</v>
       </c>
       <c r="E6" s="5" t="s">
@@ -2037,7 +2056,7 @@
       <c r="C7" s="1">
         <v>10</v>
       </c>
-      <c r="D7" s="26"/>
+      <c r="D7" s="24"/>
       <c r="E7" s="5" t="s">
         <v>17</v>
       </c>
@@ -2053,8 +2072,8 @@
       <c r="C8" s="1">
         <v>2</v>
       </c>
-      <c r="D8" s="26"/>
-      <c r="E8" s="21" t="s">
+      <c r="D8" s="24"/>
+      <c r="E8" s="27" t="s">
         <v>32</v>
       </c>
     </row>
@@ -2069,8 +2088,8 @@
       <c r="C9" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D9" s="26"/>
-      <c r="E9" s="22"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="28"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -2083,8 +2102,8 @@
       <c r="C10" s="1">
         <v>0</v>
       </c>
-      <c r="D10" s="26"/>
-      <c r="E10" s="23" t="s">
+      <c r="D10" s="24"/>
+      <c r="E10" s="29" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2099,8 +2118,8 @@
       <c r="C11" s="1">
         <v>8</v>
       </c>
-      <c r="D11" s="27"/>
-      <c r="E11" s="22"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="28"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -2326,10 +2345,10 @@
       </c>
     </row>
     <row r="5" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="24" t="s">
+      <c r="A5" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="24"/>
+      <c r="B5" s="22"/>
       <c r="C5" s="6" t="s">
         <v>4</v>
       </c>
@@ -2348,7 +2367,7 @@
       <c r="C6" s="1">
         <v>6</v>
       </c>
-      <c r="D6" s="25" t="s">
+      <c r="D6" s="23" t="s">
         <v>8</v>
       </c>
       <c r="E6" s="5" t="s">
@@ -2366,7 +2385,7 @@
       <c r="C7" s="1">
         <v>10</v>
       </c>
-      <c r="D7" s="26"/>
+      <c r="D7" s="24"/>
       <c r="E7" s="5" t="s">
         <v>31</v>
       </c>
@@ -2382,8 +2401,8 @@
       <c r="C8" s="1">
         <v>2</v>
       </c>
-      <c r="D8" s="26"/>
-      <c r="E8" s="21" t="s">
+      <c r="D8" s="24"/>
+      <c r="E8" s="27" t="s">
         <v>32</v>
       </c>
     </row>
@@ -2398,8 +2417,8 @@
       <c r="C9" s="1">
         <v>7</v>
       </c>
-      <c r="D9" s="26"/>
-      <c r="E9" s="22"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="28"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -2412,8 +2431,8 @@
       <c r="C10" s="1">
         <v>0</v>
       </c>
-      <c r="D10" s="26"/>
-      <c r="E10" s="23" t="s">
+      <c r="D10" s="24"/>
+      <c r="E10" s="29" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2428,8 +2447,8 @@
       <c r="C11" s="1">
         <v>10</v>
       </c>
-      <c r="D11" s="27"/>
-      <c r="E11" s="22"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="28"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -2478,7 +2497,7 @@
       <c r="C14" s="1">
         <v>8</v>
       </c>
-      <c r="D14" s="28" t="s">
+      <c r="D14" s="30" t="s">
         <v>9</v>
       </c>
       <c r="E14" s="5" t="s">
@@ -2496,7 +2515,7 @@
       <c r="C15" s="1">
         <v>1</v>
       </c>
-      <c r="D15" s="28"/>
+      <c r="D15" s="30"/>
       <c r="E15" s="5" t="s">
         <v>33</v>
       </c>
@@ -2512,8 +2531,8 @@
       <c r="C16" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D16" s="28"/>
-      <c r="E16" s="20" t="s">
+      <c r="D16" s="30"/>
+      <c r="E16" s="26" t="s">
         <v>12</v>
       </c>
     </row>
@@ -2528,8 +2547,8 @@
       <c r="C17" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D17" s="28"/>
-      <c r="E17" s="20"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="26"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
@@ -2542,8 +2561,8 @@
       <c r="C18" s="1">
         <v>0</v>
       </c>
-      <c r="D18" s="28"/>
-      <c r="E18" s="20"/>
+      <c r="D18" s="30"/>
+      <c r="E18" s="26"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
@@ -2556,8 +2575,8 @@
       <c r="C19" s="1">
         <v>12</v>
       </c>
-      <c r="D19" s="28"/>
-      <c r="E19" s="20"/>
+      <c r="D19" s="30"/>
+      <c r="E19" s="26"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
@@ -2570,8 +2589,8 @@
       <c r="C20" s="1">
         <v>46</v>
       </c>
-      <c r="D20" s="28"/>
-      <c r="E20" s="20" t="s">
+      <c r="D20" s="30"/>
+      <c r="E20" s="26" t="s">
         <v>13</v>
       </c>
     </row>
@@ -2586,8 +2605,8 @@
       <c r="C21" s="1">
         <v>51</v>
       </c>
-      <c r="D21" s="28"/>
-      <c r="E21" s="20"/>
+      <c r="D21" s="30"/>
+      <c r="E21" s="26"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="8"/>
@@ -2679,10 +2698,10 @@
       </c>
     </row>
     <row r="5" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="24" t="s">
+      <c r="A5" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="24"/>
+      <c r="B5" s="22"/>
       <c r="C5" s="6" t="s">
         <v>4</v>
       </c>
@@ -2701,7 +2720,7 @@
       <c r="C6" s="1">
         <v>6</v>
       </c>
-      <c r="D6" s="25" t="s">
+      <c r="D6" s="23" t="s">
         <v>8</v>
       </c>
       <c r="E6" s="5" t="s">
@@ -2719,7 +2738,7 @@
       <c r="C7" s="1">
         <v>10</v>
       </c>
-      <c r="D7" s="26"/>
+      <c r="D7" s="24"/>
       <c r="E7" s="5" t="s">
         <v>17</v>
       </c>
@@ -2735,8 +2754,8 @@
       <c r="C8" s="1">
         <v>2</v>
       </c>
-      <c r="D8" s="26"/>
-      <c r="E8" s="21" t="s">
+      <c r="D8" s="24"/>
+      <c r="E8" s="27" t="s">
         <v>32</v>
       </c>
     </row>
@@ -2751,8 +2770,8 @@
       <c r="C9" s="1">
         <v>8</v>
       </c>
-      <c r="D9" s="26"/>
-      <c r="E9" s="22"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="28"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -2765,8 +2784,8 @@
       <c r="C10" s="1">
         <v>0</v>
       </c>
-      <c r="D10" s="26"/>
-      <c r="E10" s="23" t="s">
+      <c r="D10" s="24"/>
+      <c r="E10" s="29" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2781,8 +2800,8 @@
       <c r="C11" s="1">
         <v>8</v>
       </c>
-      <c r="D11" s="27"/>
-      <c r="E11" s="22"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="28"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -2988,8 +3007,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:M31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3008,14 +3027,14 @@
   <sheetData>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>38</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="24" t="s">
+      <c r="A5" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="24"/>
+      <c r="B5" s="22"/>
       <c r="C5" s="6" t="s">
         <v>4</v>
       </c>
@@ -3034,7 +3053,7 @@
       <c r="C6" s="1">
         <v>6</v>
       </c>
-      <c r="D6" s="25" t="s">
+      <c r="D6" s="23" t="s">
         <v>8</v>
       </c>
       <c r="E6" s="5" t="s">
@@ -3061,7 +3080,7 @@
       <c r="C7" s="1">
         <v>10</v>
       </c>
-      <c r="D7" s="26"/>
+      <c r="D7" s="24"/>
       <c r="E7" s="5" t="s">
         <v>31</v>
       </c>
@@ -3086,8 +3105,8 @@
       <c r="C8" s="1">
         <v>4</v>
       </c>
-      <c r="D8" s="26"/>
-      <c r="E8" s="21" t="s">
+      <c r="D8" s="24"/>
+      <c r="E8" s="27" t="s">
         <v>32</v>
       </c>
       <c r="G8" s="1">
@@ -3111,8 +3130,8 @@
       <c r="C9" s="1">
         <v>20</v>
       </c>
-      <c r="D9" s="26"/>
-      <c r="E9" s="22"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="28"/>
       <c r="G9" s="1">
         <v>20</v>
       </c>
@@ -3134,8 +3153,8 @@
       <c r="C10" s="1">
         <v>0</v>
       </c>
-      <c r="D10" s="26"/>
-      <c r="E10" s="23" t="s">
+      <c r="D10" s="24"/>
+      <c r="E10" s="29" t="s">
         <v>18</v>
       </c>
       <c r="G10" s="1">
@@ -3159,15 +3178,15 @@
       <c r="C11" s="1">
         <v>17</v>
       </c>
-      <c r="D11" s="27"/>
-      <c r="E11" s="22"/>
-      <c r="G11" s="30">
+      <c r="D11" s="25"/>
+      <c r="E11" s="28"/>
+      <c r="G11" s="21">
         <v>17</v>
       </c>
-      <c r="H11" s="30">
+      <c r="H11" s="21">
         <v>18</v>
       </c>
-      <c r="I11" s="30">
+      <c r="I11" s="21">
         <v>15</v>
       </c>
     </row>
@@ -3182,7 +3201,7 @@
       <c r="C12" s="1">
         <v>4</v>
       </c>
-      <c r="D12" s="25" t="s">
+      <c r="D12" s="23" t="s">
         <v>47</v>
       </c>
       <c r="E12" s="3" t="s">
@@ -3209,7 +3228,7 @@
       <c r="C13" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D13" s="26"/>
+      <c r="D13" s="24"/>
       <c r="E13" s="3" t="s">
         <v>25</v>
       </c>
@@ -3234,17 +3253,17 @@
       <c r="C14" s="1">
         <v>94</v>
       </c>
-      <c r="D14" s="26"/>
+      <c r="D14" s="24"/>
       <c r="E14" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="G14" s="30">
-        <v>0</v>
-      </c>
-      <c r="H14" s="30">
+      <c r="G14" s="21">
+        <v>0</v>
+      </c>
+      <c r="H14" s="21">
         <v>3</v>
       </c>
-      <c r="I14" s="30">
+      <c r="I14" s="21">
         <v>6</v>
       </c>
     </row>
@@ -3259,8 +3278,10 @@
       <c r="C15" s="1">
         <v>0</v>
       </c>
-      <c r="D15" s="27"/>
-      <c r="E15" s="3"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="3" t="s">
+        <v>59</v>
+      </c>
       <c r="G15" s="1">
         <v>0</v>
       </c>
@@ -3282,7 +3303,7 @@
       <c r="C16" s="1">
         <v>29</v>
       </c>
-      <c r="D16" s="25" t="s">
+      <c r="D16" s="23" t="s">
         <v>46</v>
       </c>
       <c r="E16" s="19" t="s">
@@ -3309,7 +3330,7 @@
       <c r="C17" s="1">
         <v>0</v>
       </c>
-      <c r="D17" s="26"/>
+      <c r="D17" s="24"/>
       <c r="E17" s="5" t="s">
         <v>52</v>
       </c>
@@ -3334,7 +3355,7 @@
       <c r="C18" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D18" s="26"/>
+      <c r="D18" s="24"/>
       <c r="E18" s="5" t="s">
         <v>50</v>
       </c>
@@ -3359,7 +3380,7 @@
       <c r="C19" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D19" s="26"/>
+      <c r="D19" s="24"/>
       <c r="E19" s="5" t="s">
         <v>51</v>
       </c>
@@ -3384,17 +3405,17 @@
       <c r="C20" s="1">
         <v>11</v>
       </c>
-      <c r="D20" s="26"/>
-      <c r="E20" s="20" t="s">
+      <c r="D20" s="24"/>
+      <c r="E20" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="G20" s="30">
+      <c r="G20" s="21">
         <v>11</v>
       </c>
-      <c r="H20" s="30">
+      <c r="H20" s="21">
         <v>11</v>
       </c>
-      <c r="I20" s="30">
+      <c r="I20" s="21">
         <v>11</v>
       </c>
     </row>
@@ -3409,15 +3430,15 @@
       <c r="C21" s="1">
         <v>67</v>
       </c>
-      <c r="D21" s="26"/>
-      <c r="E21" s="20"/>
-      <c r="G21" s="30">
+      <c r="D21" s="24"/>
+      <c r="E21" s="26"/>
+      <c r="G21" s="21">
         <v>67</v>
       </c>
-      <c r="H21" s="30">
+      <c r="H21" s="21">
         <v>68</v>
       </c>
-      <c r="I21" s="30">
+      <c r="I21" s="21">
         <v>16</v>
       </c>
       <c r="K21" s="8"/>
@@ -3435,17 +3456,17 @@
       <c r="C22" s="1">
         <v>28</v>
       </c>
-      <c r="D22" s="26"/>
-      <c r="E22" s="20" t="s">
+      <c r="D22" s="24"/>
+      <c r="E22" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="G22" s="30">
+      <c r="G22" s="21">
         <v>28</v>
       </c>
-      <c r="H22" s="30">
+      <c r="H22" s="21">
         <v>20</v>
       </c>
-      <c r="I22" s="30">
+      <c r="I22" s="21">
         <v>0</v>
       </c>
       <c r="K22" s="8"/>
@@ -3463,15 +3484,15 @@
       <c r="C23" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D23" s="26"/>
-      <c r="E23" s="20"/>
-      <c r="G23" s="30" t="s">
+      <c r="D23" s="24"/>
+      <c r="E23" s="26"/>
+      <c r="G23" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="H23" s="30">
+      <c r="H23" s="21">
         <v>1</v>
       </c>
-      <c r="I23" s="30">
+      <c r="I23" s="21">
         <v>2</v>
       </c>
       <c r="K23" s="8"/>
@@ -3489,17 +3510,17 @@
       <c r="C24" s="1">
         <v>3</v>
       </c>
-      <c r="D24" s="26"/>
+      <c r="D24" s="24"/>
       <c r="E24" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="G24" s="30">
+      <c r="G24" s="21">
         <v>3</v>
       </c>
-      <c r="H24" s="30">
-        <v>4</v>
-      </c>
-      <c r="I24" s="30">
+      <c r="H24" s="21">
+        <v>4</v>
+      </c>
+      <c r="I24" s="21">
         <v>1</v>
       </c>
       <c r="K24" s="8"/>
@@ -3517,8 +3538,8 @@
       <c r="C25" s="1">
         <v>0</v>
       </c>
-      <c r="D25" s="26"/>
-      <c r="E25" s="20" t="s">
+      <c r="D25" s="24"/>
+      <c r="E25" s="26" t="s">
         <v>55</v>
       </c>
       <c r="G25" s="1">
@@ -3545,15 +3566,15 @@
       <c r="C26" s="1">
         <v>80</v>
       </c>
-      <c r="D26" s="26"/>
-      <c r="E26" s="20"/>
-      <c r="G26" s="30">
+      <c r="D26" s="24"/>
+      <c r="E26" s="26"/>
+      <c r="G26" s="21">
         <v>80</v>
       </c>
-      <c r="H26" s="30">
+      <c r="H26" s="21">
         <v>80</v>
       </c>
-      <c r="I26" s="30">
+      <c r="I26" s="21">
         <v>81</v>
       </c>
       <c r="K26" s="8"/>
@@ -3571,14 +3592,14 @@
       <c r="C27" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D27" s="26"/>
-      <c r="E27" s="29" t="s">
+      <c r="D27" s="24"/>
+      <c r="E27" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="G27" s="30">
+      <c r="G27" s="21">
         <v>3</v>
       </c>
-      <c r="H27" s="30">
+      <c r="H27" s="21">
         <v>15</v>
       </c>
       <c r="I27" s="1"/>
@@ -3597,12 +3618,12 @@
       <c r="C28" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D28" s="27"/>
-      <c r="E28" s="29"/>
-      <c r="G28" s="30" t="s">
+      <c r="D28" s="25"/>
+      <c r="E28" s="31"/>
+      <c r="G28" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="H28" s="30" t="s">
+      <c r="H28" s="21" t="s">
         <v>0</v>
       </c>
       <c r="I28" s="1"/>
@@ -3621,8 +3642,8 @@
       <c r="C29" s="1"/>
       <c r="D29" s="9"/>
       <c r="E29" s="10"/>
-      <c r="G29" s="30"/>
-      <c r="H29" s="30">
+      <c r="G29" s="21"/>
+      <c r="H29" s="21">
         <v>0</v>
       </c>
       <c r="I29" s="1"/>
@@ -3646,22 +3667,701 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="D12:D15"/>
+    <mergeCell ref="D16:D28"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="D6:D11"/>
     <mergeCell ref="E8:E9"/>
     <mergeCell ref="E10:E11"/>
     <mergeCell ref="E20:E21"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="D12:D15"/>
-    <mergeCell ref="D16:D28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:M31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.5703125" customWidth="1"/>
+    <col min="2" max="2" width="6.140625" customWidth="1"/>
+    <col min="3" max="3" width="6.28515625" style="7" customWidth="1"/>
+    <col min="4" max="4" width="4.5703125" customWidth="1"/>
+    <col min="5" max="5" width="55.42578125" customWidth="1"/>
+    <col min="6" max="6" width="2.140625" customWidth="1"/>
+    <col min="7" max="9" width="4.140625" customWidth="1"/>
+    <col min="10" max="12" width="4.5703125" customWidth="1"/>
+    <col min="13" max="13" width="33.140625" customWidth="1"/>
+    <col min="14" max="26" width="4.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="22"/>
+      <c r="C5" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6" s="7" t="str">
+        <f>CONCATENATE("0x",DEC2HEX(A6,2))</f>
+        <v>0x01</v>
+      </c>
+      <c r="C6" s="1">
+        <v>6</v>
+      </c>
+      <c r="D6" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" s="1">
+        <v>6</v>
+      </c>
+      <c r="H6" s="1">
+        <v>6</v>
+      </c>
+      <c r="I6" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7" s="7" t="str">
+        <f t="shared" ref="B7:B29" si="0">CONCATENATE("0x",DEC2HEX(A7,2))</f>
+        <v>0x02</v>
+      </c>
+      <c r="C7" s="1">
+        <v>10</v>
+      </c>
+      <c r="D7" s="24"/>
+      <c r="E7" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="G7" s="1">
+        <v>10</v>
+      </c>
+      <c r="H7" s="1">
+        <v>10</v>
+      </c>
+      <c r="I7" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>0x03</v>
+      </c>
+      <c r="C8" s="1">
+        <v>4</v>
+      </c>
+      <c r="D8" s="24"/>
+      <c r="E8" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="G8" s="1">
+        <v>4</v>
+      </c>
+      <c r="H8" s="1">
+        <v>4</v>
+      </c>
+      <c r="I8" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="261" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="16">
+        <v>4</v>
+      </c>
+      <c r="B9" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v>0x04</v>
+      </c>
+      <c r="C9" s="1">
+        <v>20</v>
+      </c>
+      <c r="D9" s="24"/>
+      <c r="E9" s="28"/>
+      <c r="G9" s="1">
+        <v>20</v>
+      </c>
+      <c r="H9" s="1">
+        <v>20</v>
+      </c>
+      <c r="I9" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>5</v>
+      </c>
+      <c r="B10" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>0x05</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0</v>
+      </c>
+      <c r="D10" s="24"/>
+      <c r="E10" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" s="1">
+        <v>0</v>
+      </c>
+      <c r="H10" s="1">
+        <v>0</v>
+      </c>
+      <c r="I10" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>6</v>
+      </c>
+      <c r="B11" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>0x06</v>
+      </c>
+      <c r="C11" s="1">
+        <v>17</v>
+      </c>
+      <c r="D11" s="25"/>
+      <c r="E11" s="28"/>
+      <c r="G11" s="21">
+        <v>17</v>
+      </c>
+      <c r="H11" s="21">
+        <v>18</v>
+      </c>
+      <c r="I11" s="21">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>7</v>
+      </c>
+      <c r="B12" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>0x07</v>
+      </c>
+      <c r="C12" s="1">
+        <v>4</v>
+      </c>
+      <c r="D12" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G12" s="1">
+        <v>4</v>
+      </c>
+      <c r="H12" s="1">
+        <v>4</v>
+      </c>
+      <c r="I12" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>8</v>
+      </c>
+      <c r="B13" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>0x08</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="24"/>
+      <c r="E13" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G13" s="1">
+        <v>48</v>
+      </c>
+      <c r="H13" s="1">
+        <v>48</v>
+      </c>
+      <c r="I13" s="1">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>9</v>
+      </c>
+      <c r="B14" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>0x09</v>
+      </c>
+      <c r="C14" s="1">
+        <v>94</v>
+      </c>
+      <c r="D14" s="24"/>
+      <c r="E14" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G14" s="21">
+        <v>0</v>
+      </c>
+      <c r="H14" s="21">
+        <v>3</v>
+      </c>
+      <c r="I14" s="21">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>10</v>
+      </c>
+      <c r="B15" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>0x0A</v>
+      </c>
+      <c r="C15" s="1">
+        <v>0</v>
+      </c>
+      <c r="D15" s="25"/>
+      <c r="E15" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G15" s="1">
+        <v>0</v>
+      </c>
+      <c r="H15" s="1">
+        <v>0</v>
+      </c>
+      <c r="I15" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>11</v>
+      </c>
+      <c r="B16" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>0x0B</v>
+      </c>
+      <c r="C16" s="1">
+        <v>11</v>
+      </c>
+      <c r="D16" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="E16" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="G16" s="1">
+        <v>11</v>
+      </c>
+      <c r="H16" s="1">
+        <v>11</v>
+      </c>
+      <c r="I16" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>12</v>
+      </c>
+      <c r="B17" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>0x0C</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0</v>
+      </c>
+      <c r="D17" s="24"/>
+      <c r="E17" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="G17" s="1">
+        <v>0</v>
+      </c>
+      <c r="H17" s="1">
+        <v>0</v>
+      </c>
+      <c r="I17" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>13</v>
+      </c>
+      <c r="B18" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>0x0D</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" s="24"/>
+      <c r="E18" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>14</v>
+      </c>
+      <c r="B19" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>0x0E</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D19" s="24"/>
+      <c r="E19" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>15</v>
+      </c>
+      <c r="B20" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>0x0F</v>
+      </c>
+      <c r="C20" s="1">
+        <v>11</v>
+      </c>
+      <c r="D20" s="24"/>
+      <c r="E20" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="G20" s="21">
+        <v>11</v>
+      </c>
+      <c r="H20" s="21">
+        <v>11</v>
+      </c>
+      <c r="I20" s="21">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>16</v>
+      </c>
+      <c r="B21" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>0x10</v>
+      </c>
+      <c r="C21" s="1">
+        <v>67</v>
+      </c>
+      <c r="D21" s="24"/>
+      <c r="E21" s="26"/>
+      <c r="G21" s="21">
+        <v>67</v>
+      </c>
+      <c r="H21" s="21">
+        <v>68</v>
+      </c>
+      <c r="I21" s="21">
+        <v>16</v>
+      </c>
+      <c r="K21" s="8"/>
+      <c r="L21" s="8"/>
+      <c r="M21" s="8"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>17</v>
+      </c>
+      <c r="B22" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>0x11</v>
+      </c>
+      <c r="C22" s="1">
+        <v>28</v>
+      </c>
+      <c r="D22" s="24"/>
+      <c r="E22" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="G22" s="21">
+        <v>28</v>
+      </c>
+      <c r="H22" s="21">
+        <v>20</v>
+      </c>
+      <c r="I22" s="21">
+        <v>0</v>
+      </c>
+      <c r="K22" s="8"/>
+      <c r="L22" s="9"/>
+      <c r="M22" s="10"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>18</v>
+      </c>
+      <c r="B23" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>0x12</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D23" s="24"/>
+      <c r="E23" s="26"/>
+      <c r="G23" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="H23" s="21">
+        <v>1</v>
+      </c>
+      <c r="I23" s="21">
+        <v>2</v>
+      </c>
+      <c r="K23" s="8"/>
+      <c r="L23" s="9"/>
+      <c r="M23" s="10"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>19</v>
+      </c>
+      <c r="B24" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>0x13</v>
+      </c>
+      <c r="C24" s="1">
+        <v>3</v>
+      </c>
+      <c r="D24" s="24"/>
+      <c r="E24" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="G24" s="21">
+        <v>3</v>
+      </c>
+      <c r="H24" s="21">
+        <v>4</v>
+      </c>
+      <c r="I24" s="21">
+        <v>1</v>
+      </c>
+      <c r="K24" s="8"/>
+      <c r="L24" s="9"/>
+      <c r="M24" s="12"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>20</v>
+      </c>
+      <c r="B25" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>0x14</v>
+      </c>
+      <c r="C25" s="1">
+        <v>0</v>
+      </c>
+      <c r="D25" s="24"/>
+      <c r="E25" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="G25" s="1">
+        <v>0</v>
+      </c>
+      <c r="H25" s="1">
+        <v>0</v>
+      </c>
+      <c r="I25" s="1">
+        <v>0</v>
+      </c>
+      <c r="K25" s="8"/>
+      <c r="L25" s="9"/>
+      <c r="M25" s="12"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>21</v>
+      </c>
+      <c r="B26" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>0x15</v>
+      </c>
+      <c r="C26" s="1">
+        <v>80</v>
+      </c>
+      <c r="D26" s="24"/>
+      <c r="E26" s="26"/>
+      <c r="G26" s="21">
+        <v>80</v>
+      </c>
+      <c r="H26" s="21">
+        <v>80</v>
+      </c>
+      <c r="I26" s="21">
+        <v>81</v>
+      </c>
+      <c r="K26" s="8"/>
+      <c r="L26" s="9"/>
+      <c r="M26" s="12"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>22</v>
+      </c>
+      <c r="B27" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>0x16</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D27" s="24"/>
+      <c r="E27" s="31" t="s">
+        <v>56</v>
+      </c>
+      <c r="G27" s="21">
+        <v>3</v>
+      </c>
+      <c r="H27" s="21">
+        <v>15</v>
+      </c>
+      <c r="I27" s="1"/>
+      <c r="K27" s="8"/>
+      <c r="L27" s="9"/>
+      <c r="M27" s="12"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>23</v>
+      </c>
+      <c r="B28" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>0x17</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D28" s="25"/>
+      <c r="E28" s="31"/>
+      <c r="G28" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="H28" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="I28" s="1"/>
+      <c r="K28" s="8"/>
+      <c r="L28" s="9"/>
+      <c r="M28" s="12"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>24</v>
+      </c>
+      <c r="B29" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>0x18</v>
+      </c>
+      <c r="C29" s="1"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="10"/>
+      <c r="G29" s="21"/>
+      <c r="H29" s="21">
+        <v>0</v>
+      </c>
+      <c r="I29" s="1"/>
+      <c r="K29" s="8"/>
+      <c r="L29" s="9"/>
+      <c r="M29" s="12"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B30" s="7"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="10"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B31" s="7"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="10"/>
+      <c r="F31" s="12"/>
+      <c r="G31" s="18"/>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="D6:D11"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="D12:D15"/>
+    <mergeCell ref="D16:D28"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="E27:E28"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:Y30"/>
   <sheetViews>

</xml_diff>